<commit_message>
Feat: Atualizei o motor de validação, fiz vários ajustes visuais
</commit_message>
<xml_diff>
--- a/app/development/catalogo/data/catalogo_codigos.xlsx
+++ b/app/development/catalogo/data/catalogo_codigos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="908">
   <si>
     <t xml:space="preserve">CÓDIGO</t>
   </si>
@@ -2714,6 +2714,36 @@
   </si>
   <si>
     <t xml:space="preserve">CONDENSADOR AWS-C-24QF 220V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL0124-0082-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI PRINCIPAL CM-550-L - MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL0224-0079-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI DISPLAY CM-400-L - IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL0224-0081-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI FONTE CM-400L - IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL0224-0089-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI DISPLAY CM-700/CM-1000N - IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL0224-0092-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCI DISPLAY CM-550-L - IM</t>
   </si>
 </sst>
 </file>
@@ -2844,8 +2874,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A688" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B710" activeCellId="0" sqref="B710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10556,7 +10586,61 @@
         <v>849</v>
       </c>
     </row>
-    <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A701" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B701" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C701" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A702" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B702" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C702" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="B703" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C703" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B704" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C704" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B705" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C705" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>